<commit_message>
Create SHS example B - CIFMM-2304
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/patient-dh-base-1.xlsx
+++ b/output/SharedHealthSummary/patient-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$242</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$240</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8745" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8668" uniqueCount="684">
   <si>
     <t>Path</t>
   </si>
@@ -1512,37 +1512,35 @@
     <t>The fact that a patient is deceased influences the clinical process. Also, in human communication and relation management it is necessary to know whether the person is alive.</t>
   </si>
   <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/deceasedInd, player[classCode=PSN|ANM and determinerCode=INSTANCE]/deceasedTime</t>
   </si>
   <si>
     <t>PID-30  (bool) and PID-29 (datetime)</t>
   </si>
   <si>
+    <t>Patient.deceasedBoolean</t>
+  </si>
+  <si>
     <t>deceasedBoolean</t>
   </si>
   <si>
     <t>Boolean indicates if individual is deceased</t>
   </si>
   <si>
+    <t>Boolean indicator if the individual is deceased or not.</t>
+  </si>
+  <si>
+    <t>Patient.deceasedDateTime</t>
+  </si>
+  <si>
     <t>deceasedDateTime</t>
   </si>
   <si>
     <t>Indicates date-time the individual died</t>
-  </si>
-  <si>
-    <t>Patient.deceasedBoolean</t>
-  </si>
-  <si>
-    <t>Deceased Indicator</t>
-  </si>
-  <si>
-    <t>Boolean indicator if the individual is deceased or not.</t>
-  </si>
-  <si>
-    <t>Patient.deceasedDateTime</t>
-  </si>
-  <si>
-    <t>Deceased Date Time</t>
   </si>
   <si>
     <t>Indivdual deceased date-time with optional accuracy indicator.</t>
@@ -2285,7 +2283,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO242"/>
+  <dimension ref="A1:AO240"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -12160,7 +12158,7 @@
       </c>
       <c r="D87" s="2"/>
       <c r="E87" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F87" t="s" s="2">
         <v>52</v>
@@ -12502,7 +12500,7 @@
       </c>
       <c r="D90" s="2"/>
       <c r="E90" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F90" t="s" s="2">
         <v>52</v>
@@ -14446,7 +14444,7 @@
       </c>
       <c r="D107" s="2"/>
       <c r="E107" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F107" t="s" s="2">
         <v>52</v>
@@ -14788,7 +14786,7 @@
       </c>
       <c r="D110" s="2"/>
       <c r="E110" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F110" t="s" s="2">
         <v>52</v>
@@ -16732,7 +16730,7 @@
       </c>
       <c r="D127" s="2"/>
       <c r="E127" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F127" t="s" s="2">
         <v>52</v>
@@ -17074,7 +17072,7 @@
       </c>
       <c r="D130" s="2"/>
       <c r="E130" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F130" t="s" s="2">
         <v>52</v>
@@ -24836,7 +24834,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
         <v>476</v>
       </c>
@@ -24910,16 +24908,14 @@
         <v>44</v>
       </c>
       <c r="AA198" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB198" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>482</v>
+      </c>
+      <c r="AB198" s="2"/>
       <c r="AC198" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD198" t="s" s="2">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="AE198" t="s" s="2">
         <v>476</v>
@@ -24937,7 +24933,7 @@
         <v>44</v>
       </c>
       <c r="AJ198" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AK198" t="s" s="2">
         <v>147</v>
@@ -24946,7 +24942,7 @@
         <v>44</v>
       </c>
       <c r="AM198" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AN198" t="s" s="2">
         <v>44</v>
@@ -24954,10 +24950,10 @@
     </row>
     <row r="199">
       <c r="A199" t="s" s="2">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="B199" t="s" s="2">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C199" t="s" s="2">
         <v>44</v>
@@ -24979,13 +24975,13 @@
         <v>53</v>
       </c>
       <c r="J199" t="s" s="2">
-        <v>477</v>
+        <v>245</v>
       </c>
       <c r="K199" t="s" s="2">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="L199" t="s" s="2">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="M199" t="s" s="2">
         <v>480</v>
@@ -25055,7 +25051,7 @@
         <v>44</v>
       </c>
       <c r="AJ199" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AK199" t="s" s="2">
         <v>147</v>
@@ -25064,7 +25060,7 @@
         <v>44</v>
       </c>
       <c r="AM199" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AN199" t="s" s="2">
         <v>44</v>
@@ -25072,10 +25068,10 @@
     </row>
     <row r="200">
       <c r="A200" t="s" s="2">
-        <v>476</v>
+        <v>489</v>
       </c>
       <c r="B200" t="s" s="2">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C200" t="s" s="2">
         <v>44</v>
@@ -25097,13 +25093,13 @@
         <v>53</v>
       </c>
       <c r="J200" t="s" s="2">
-        <v>477</v>
+        <v>313</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="L200" t="s" s="2">
-        <v>479</v>
+        <v>492</v>
       </c>
       <c r="M200" t="s" s="2">
         <v>480</v>
@@ -25173,7 +25169,7 @@
         <v>44</v>
       </c>
       <c r="AJ200" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AK200" t="s" s="2">
         <v>147</v>
@@ -25182,7 +25178,7 @@
         <v>44</v>
       </c>
       <c r="AM200" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AN200" t="s" s="2">
         <v>44</v>
@@ -25190,11 +25186,9 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="B201" t="s" s="2">
-        <v>484</v>
-      </c>
+        <v>493</v>
+      </c>
+      <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
         <v>44</v>
       </c>
@@ -25209,26 +25203,22 @@
         <v>44</v>
       </c>
       <c r="H201" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I201" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J201" t="s" s="2">
-        <v>245</v>
+        <v>143</v>
       </c>
       <c r="K201" t="s" s="2">
-        <v>489</v>
+        <v>144</v>
       </c>
       <c r="L201" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="M201" t="s" s="2">
-        <v>480</v>
-      </c>
-      <c r="N201" t="s" s="2">
-        <v>481</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="M201" s="2"/>
+      <c r="N201" s="2"/>
       <c r="O201" t="s" s="2">
         <v>44</v>
       </c>
@@ -25276,7 +25266,7 @@
         <v>44</v>
       </c>
       <c r="AE201" t="s" s="2">
-        <v>476</v>
+        <v>146</v>
       </c>
       <c r="AF201" t="s" s="2">
         <v>42</v>
@@ -25291,16 +25281,16 @@
         <v>44</v>
       </c>
       <c r="AJ201" t="s" s="2">
-        <v>482</v>
+        <v>44</v>
       </c>
       <c r="AK201" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL201" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM201" t="s" s="2">
-        <v>483</v>
+        <v>44</v>
       </c>
       <c r="AN201" t="s" s="2">
         <v>44</v>
@@ -25308,11 +25298,9 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>491</v>
-      </c>
-      <c r="B202" t="s" s="2">
-        <v>486</v>
-      </c>
+        <v>494</v>
+      </c>
+      <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
         <v>44</v>
       </c>
@@ -25321,32 +25309,28 @@
         <v>42</v>
       </c>
       <c r="F202" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G202" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H202" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I202" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J202" t="s" s="2">
-        <v>313</v>
+        <v>97</v>
       </c>
       <c r="K202" t="s" s="2">
-        <v>492</v>
+        <v>98</v>
       </c>
       <c r="L202" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="M202" t="s" s="2">
-        <v>480</v>
-      </c>
-      <c r="N202" t="s" s="2">
-        <v>481</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M202" s="2"/>
+      <c r="N202" s="2"/>
       <c r="O202" t="s" s="2">
         <v>44</v>
       </c>
@@ -25382,25 +25366,23 @@
         <v>44</v>
       </c>
       <c r="AA202" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB202" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="AB202" s="2"/>
       <c r="AC202" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD202" t="s" s="2">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="AE202" t="s" s="2">
-        <v>476</v>
+        <v>150</v>
       </c>
       <c r="AF202" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG202" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH202" t="s" s="2">
         <v>44</v>
@@ -25409,16 +25391,16 @@
         <v>44</v>
       </c>
       <c r="AJ202" t="s" s="2">
-        <v>482</v>
+        <v>44</v>
       </c>
       <c r="AK202" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL202" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM202" t="s" s="2">
-        <v>483</v>
+        <v>44</v>
       </c>
       <c r="AN202" t="s" s="2">
         <v>44</v>
@@ -25428,7 +25410,9 @@
       <c r="A203" t="s" s="2">
         <v>494</v>
       </c>
-      <c r="B203" s="2"/>
+      <c r="B203" t="s" s="2">
+        <v>462</v>
+      </c>
       <c r="C203" t="s" s="2">
         <v>44</v>
       </c>
@@ -25449,15 +25433,17 @@
         <v>44</v>
       </c>
       <c r="J203" t="s" s="2">
-        <v>143</v>
+        <v>463</v>
       </c>
       <c r="K203" t="s" s="2">
-        <v>144</v>
+        <v>495</v>
       </c>
       <c r="L203" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="M203" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="M203" t="s" s="2">
+        <v>496</v>
+      </c>
       <c r="N203" s="2"/>
       <c r="O203" t="s" s="2">
         <v>44</v>
@@ -25506,19 +25492,19 @@
         <v>44</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG203" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH203" t="s" s="2">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="AI203" t="s" s="2">
-        <v>44</v>
+        <v>497</v>
       </c>
       <c r="AJ203" t="s" s="2">
         <v>44</v>
@@ -25538,7 +25524,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -25549,7 +25535,7 @@
         <v>42</v>
       </c>
       <c r="F204" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G204" t="s" s="2">
         <v>44</v>
@@ -25561,13 +25547,13 @@
         <v>44</v>
       </c>
       <c r="J204" t="s" s="2">
-        <v>97</v>
+        <v>472</v>
       </c>
       <c r="K204" t="s" s="2">
-        <v>98</v>
+        <v>499</v>
       </c>
       <c r="L204" t="s" s="2">
-        <v>99</v>
+        <v>474</v>
       </c>
       <c r="M204" s="2"/>
       <c r="N204" s="2"/>
@@ -25606,23 +25592,25 @@
         <v>44</v>
       </c>
       <c r="AA204" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AB204" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB204" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC204" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD204" t="s" s="2">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG204" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH204" t="s" s="2">
         <v>44</v>
@@ -25646,13 +25634,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="205" hidden="true">
+    <row r="205">
       <c r="A205" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="B205" t="s" s="2">
-        <v>462</v>
-      </c>
+        <v>501</v>
+      </c>
+      <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
         <v>44</v>
       </c>
@@ -25661,30 +25647,32 @@
         <v>42</v>
       </c>
       <c r="F205" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G205" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H205" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I205" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J205" t="s" s="2">
-        <v>463</v>
+        <v>502</v>
       </c>
       <c r="K205" t="s" s="2">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="L205" t="s" s="2">
-        <v>465</v>
+        <v>504</v>
       </c>
       <c r="M205" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="N205" s="2"/>
+        <v>505</v>
+      </c>
+      <c r="N205" t="s" s="2">
+        <v>506</v>
+      </c>
       <c r="O205" t="s" s="2">
         <v>44</v>
       </c>
@@ -25732,7 +25720,7 @@
         <v>44</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>150</v>
+        <v>501</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>42</v>
@@ -25741,30 +25729,30 @@
         <v>43</v>
       </c>
       <c r="AH205" t="s" s="2">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="AI205" t="s" s="2">
-        <v>498</v>
+        <v>44</v>
       </c>
       <c r="AJ205" t="s" s="2">
-        <v>44</v>
+        <v>507</v>
       </c>
       <c r="AK205" t="s" s="2">
-        <v>44</v>
+        <v>508</v>
       </c>
       <c r="AL205" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM205" t="s" s="2">
-        <v>44</v>
+        <v>509</v>
       </c>
       <c r="AN205" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="206" hidden="true">
+    <row r="206">
       <c r="A206" t="s" s="2">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" t="s" s="2">
@@ -25778,7 +25766,7 @@
         <v>52</v>
       </c>
       <c r="G206" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H206" t="s" s="2">
         <v>44</v>
@@ -25787,16 +25775,18 @@
         <v>44</v>
       </c>
       <c r="J206" t="s" s="2">
-        <v>472</v>
+        <v>192</v>
       </c>
       <c r="K206" t="s" s="2">
-        <v>500</v>
+        <v>511</v>
       </c>
       <c r="L206" t="s" s="2">
-        <v>474</v>
+        <v>512</v>
       </c>
       <c r="M206" s="2"/>
-      <c r="N206" s="2"/>
+      <c r="N206" t="s" s="2">
+        <v>513</v>
+      </c>
       <c r="O206" t="s" s="2">
         <v>44</v>
       </c>
@@ -25820,13 +25810,13 @@
         <v>44</v>
       </c>
       <c r="W206" t="s" s="2">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="X206" t="s" s="2">
-        <v>44</v>
+        <v>514</v>
       </c>
       <c r="Y206" t="s" s="2">
-        <v>44</v>
+        <v>515</v>
       </c>
       <c r="Z206" t="s" s="2">
         <v>44</v>
@@ -25844,7 +25834,7 @@
         <v>44</v>
       </c>
       <c r="AE206" t="s" s="2">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="AF206" t="s" s="2">
         <v>42</v>
@@ -25859,16 +25849,16 @@
         <v>44</v>
       </c>
       <c r="AJ206" t="s" s="2">
-        <v>44</v>
+        <v>516</v>
       </c>
       <c r="AK206" t="s" s="2">
-        <v>44</v>
+        <v>517</v>
       </c>
       <c r="AL206" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM206" t="s" s="2">
-        <v>44</v>
+        <v>518</v>
       </c>
       <c r="AN206" t="s" s="2">
         <v>44</v>
@@ -25876,7 +25866,7 @@
     </row>
     <row r="207">
       <c r="A207" t="s" s="2">
-        <v>502</v>
+        <v>519</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" t="s" s="2">
@@ -25887,7 +25877,7 @@
         <v>42</v>
       </c>
       <c r="F207" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G207" t="s" s="2">
         <v>53</v>
@@ -25896,22 +25886,22 @@
         <v>44</v>
       </c>
       <c r="I207" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J207" t="s" s="2">
-        <v>503</v>
+        <v>520</v>
       </c>
       <c r="K207" t="s" s="2">
-        <v>504</v>
+        <v>521</v>
       </c>
       <c r="L207" t="s" s="2">
-        <v>505</v>
+        <v>522</v>
       </c>
       <c r="M207" t="s" s="2">
-        <v>506</v>
+        <v>523</v>
       </c>
       <c r="N207" t="s" s="2">
-        <v>507</v>
+        <v>524</v>
       </c>
       <c r="O207" t="s" s="2">
         <v>44</v>
@@ -25960,13 +25950,13 @@
         <v>44</v>
       </c>
       <c r="AE207" t="s" s="2">
-        <v>502</v>
+        <v>519</v>
       </c>
       <c r="AF207" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG207" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH207" t="s" s="2">
         <v>44</v>
@@ -25975,16 +25965,16 @@
         <v>44</v>
       </c>
       <c r="AJ207" t="s" s="2">
-        <v>508</v>
+        <v>525</v>
       </c>
       <c r="AK207" t="s" s="2">
-        <v>509</v>
+        <v>147</v>
       </c>
       <c r="AL207" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM207" t="s" s="2">
-        <v>510</v>
+        <v>526</v>
       </c>
       <c r="AN207" t="s" s="2">
         <v>44</v>
@@ -25992,7 +25982,7 @@
     </row>
     <row r="208">
       <c r="A208" t="s" s="2">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -26003,7 +25993,7 @@
         <v>42</v>
       </c>
       <c r="F208" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G208" t="s" s="2">
         <v>53</v>
@@ -26015,17 +26005,17 @@
         <v>44</v>
       </c>
       <c r="J208" t="s" s="2">
-        <v>192</v>
+        <v>528</v>
       </c>
       <c r="K208" t="s" s="2">
-        <v>512</v>
+        <v>529</v>
       </c>
       <c r="L208" t="s" s="2">
-        <v>513</v>
+        <v>530</v>
       </c>
       <c r="M208" s="2"/>
       <c r="N208" t="s" s="2">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="O208" t="s" s="2">
         <v>44</v>
@@ -26050,13 +26040,13 @@
         <v>44</v>
       </c>
       <c r="W208" t="s" s="2">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="X208" t="s" s="2">
-        <v>515</v>
+        <v>44</v>
       </c>
       <c r="Y208" t="s" s="2">
-        <v>516</v>
+        <v>44</v>
       </c>
       <c r="Z208" t="s" s="2">
         <v>44</v>
@@ -26074,13 +26064,13 @@
         <v>44</v>
       </c>
       <c r="AE208" t="s" s="2">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="AF208" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG208" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH208" t="s" s="2">
         <v>44</v>
@@ -26089,16 +26079,16 @@
         <v>44</v>
       </c>
       <c r="AJ208" t="s" s="2">
-        <v>517</v>
+        <v>532</v>
       </c>
       <c r="AK208" t="s" s="2">
-        <v>518</v>
+        <v>147</v>
       </c>
       <c r="AL208" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM208" t="s" s="2">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="AN208" t="s" s="2">
         <v>44</v>
@@ -26106,7 +26096,7 @@
     </row>
     <row r="209">
       <c r="A209" t="s" s="2">
-        <v>520</v>
+        <v>534</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -26117,7 +26107,7 @@
         <v>42</v>
       </c>
       <c r="F209" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G209" t="s" s="2">
         <v>53</v>
@@ -26129,19 +26119,19 @@
         <v>44</v>
       </c>
       <c r="J209" t="s" s="2">
-        <v>521</v>
+        <v>535</v>
       </c>
       <c r="K209" t="s" s="2">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="L209" t="s" s="2">
-        <v>523</v>
+        <v>537</v>
       </c>
       <c r="M209" t="s" s="2">
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="N209" t="s" s="2">
-        <v>525</v>
+        <v>539</v>
       </c>
       <c r="O209" t="s" s="2">
         <v>44</v>
@@ -26190,22 +26180,22 @@
         <v>44</v>
       </c>
       <c r="AE209" t="s" s="2">
-        <v>520</v>
+        <v>534</v>
       </c>
       <c r="AF209" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG209" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH209" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI209" t="s" s="2">
-        <v>44</v>
+        <v>540</v>
       </c>
       <c r="AJ209" t="s" s="2">
-        <v>526</v>
+        <v>541</v>
       </c>
       <c r="AK209" t="s" s="2">
         <v>147</v>
@@ -26214,15 +26204,15 @@
         <v>44</v>
       </c>
       <c r="AM209" t="s" s="2">
-        <v>527</v>
+        <v>44</v>
       </c>
       <c r="AN209" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -26233,10 +26223,10 @@
         <v>42</v>
       </c>
       <c r="F210" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G210" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H210" t="s" s="2">
         <v>44</v>
@@ -26245,18 +26235,16 @@
         <v>44</v>
       </c>
       <c r="J210" t="s" s="2">
-        <v>529</v>
+        <v>143</v>
       </c>
       <c r="K210" t="s" s="2">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="L210" t="s" s="2">
-        <v>531</v>
+        <v>145</v>
       </c>
       <c r="M210" s="2"/>
-      <c r="N210" t="s" s="2">
-        <v>532</v>
-      </c>
+      <c r="N210" s="2"/>
       <c r="O210" t="s" s="2">
         <v>44</v>
       </c>
@@ -26304,13 +26292,13 @@
         <v>44</v>
       </c>
       <c r="AE210" t="s" s="2">
-        <v>528</v>
+        <v>146</v>
       </c>
       <c r="AF210" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG210" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH210" t="s" s="2">
         <v>44</v>
@@ -26319,28 +26307,28 @@
         <v>44</v>
       </c>
       <c r="AJ210" t="s" s="2">
-        <v>533</v>
+        <v>147</v>
       </c>
       <c r="AK210" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL210" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM210" t="s" s="2">
-        <v>534</v>
+        <v>44</v>
       </c>
       <c r="AN210" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" t="s" s="2">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="D211" s="2"/>
       <c r="E211" t="s" s="2">
@@ -26350,7 +26338,7 @@
         <v>43</v>
       </c>
       <c r="G211" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H211" t="s" s="2">
         <v>44</v>
@@ -26359,20 +26347,18 @@
         <v>44</v>
       </c>
       <c r="J211" t="s" s="2">
-        <v>536</v>
+        <v>97</v>
       </c>
       <c r="K211" t="s" s="2">
-        <v>537</v>
+        <v>157</v>
       </c>
       <c r="L211" t="s" s="2">
-        <v>538</v>
+        <v>158</v>
       </c>
       <c r="M211" t="s" s="2">
-        <v>539</v>
-      </c>
-      <c r="N211" t="s" s="2">
-        <v>540</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="N211" s="2"/>
       <c r="O211" t="s" s="2">
         <v>44</v>
       </c>
@@ -26420,7 +26406,7 @@
         <v>44</v>
       </c>
       <c r="AE211" t="s" s="2">
-        <v>535</v>
+        <v>150</v>
       </c>
       <c r="AF211" t="s" s="2">
         <v>42</v>
@@ -26432,13 +26418,13 @@
         <v>44</v>
       </c>
       <c r="AI211" t="s" s="2">
-        <v>541</v>
+        <v>44</v>
       </c>
       <c r="AJ211" t="s" s="2">
-        <v>542</v>
+        <v>147</v>
       </c>
       <c r="AK211" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL211" t="s" s="2">
         <v>44</v>
@@ -26452,38 +26438,40 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
-        <v>44</v>
+        <v>545</v>
       </c>
       <c r="D212" s="2"/>
       <c r="E212" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F212" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G212" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H212" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I212" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J212" t="s" s="2">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="K212" t="s" s="2">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="L212" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M212" s="2"/>
+        <v>546</v>
+      </c>
+      <c r="M212" t="s" s="2">
+        <v>127</v>
+      </c>
       <c r="N212" s="2"/>
       <c r="O212" t="s" s="2">
         <v>44</v>
@@ -26532,13 +26520,13 @@
         <v>44</v>
       </c>
       <c r="AE212" t="s" s="2">
-        <v>146</v>
+        <v>547</v>
       </c>
       <c r="AF212" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG212" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH212" t="s" s="2">
         <v>44</v>
@@ -26547,7 +26535,7 @@
         <v>44</v>
       </c>
       <c r="AJ212" t="s" s="2">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="AK212" t="s" s="2">
         <v>44</v>
@@ -26562,13 +26550,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="213" hidden="true">
+    <row r="213">
       <c r="A213" t="s" s="2">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="D213" s="2"/>
       <c r="E213" t="s" s="2">
@@ -26578,7 +26566,7 @@
         <v>43</v>
       </c>
       <c r="G213" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H213" t="s" s="2">
         <v>44</v>
@@ -26587,18 +26575,18 @@
         <v>44</v>
       </c>
       <c r="J213" t="s" s="2">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="K213" t="s" s="2">
-        <v>157</v>
+        <v>549</v>
       </c>
       <c r="L213" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M213" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="N213" s="2"/>
+        <v>550</v>
+      </c>
+      <c r="M213" s="2"/>
+      <c r="N213" t="s" s="2">
+        <v>551</v>
+      </c>
       <c r="O213" t="s" s="2">
         <v>44</v>
       </c>
@@ -26622,13 +26610,11 @@
         <v>44</v>
       </c>
       <c r="W213" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X213" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="X213" s="2"/>
       <c r="Y213" t="s" s="2">
-        <v>44</v>
+        <v>552</v>
       </c>
       <c r="Z213" t="s" s="2">
         <v>44</v>
@@ -26646,7 +26632,7 @@
         <v>44</v>
       </c>
       <c r="AE213" t="s" s="2">
-        <v>150</v>
+        <v>548</v>
       </c>
       <c r="AF213" t="s" s="2">
         <v>42</v>
@@ -26661,58 +26647,58 @@
         <v>44</v>
       </c>
       <c r="AJ213" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="AK213" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="AK213" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="AL213" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM213" t="s" s="2">
-        <v>44</v>
+        <v>554</v>
       </c>
       <c r="AN213" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="214" hidden="true">
+    <row r="214">
       <c r="A214" t="s" s="2">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
-        <v>546</v>
+        <v>44</v>
       </c>
       <c r="D214" s="2"/>
       <c r="E214" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F214" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G214" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H214" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I214" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J214" t="s" s="2">
-        <v>97</v>
+        <v>421</v>
       </c>
       <c r="K214" t="s" s="2">
-        <v>125</v>
+        <v>556</v>
       </c>
       <c r="L214" t="s" s="2">
-        <v>547</v>
-      </c>
-      <c r="M214" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="N214" s="2"/>
+        <v>557</v>
+      </c>
+      <c r="M214" s="2"/>
+      <c r="N214" t="s" s="2">
+        <v>558</v>
+      </c>
       <c r="O214" t="s" s="2">
         <v>44</v>
       </c>
@@ -26760,13 +26746,13 @@
         <v>44</v>
       </c>
       <c r="AE214" t="s" s="2">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="AF214" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG214" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH214" t="s" s="2">
         <v>44</v>
@@ -26775,16 +26761,16 @@
         <v>44</v>
       </c>
       <c r="AJ214" t="s" s="2">
-        <v>95</v>
+        <v>426</v>
       </c>
       <c r="AK214" t="s" s="2">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="AL214" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM214" t="s" s="2">
-        <v>44</v>
+        <v>559</v>
       </c>
       <c r="AN214" t="s" s="2">
         <v>44</v>
@@ -26792,7 +26778,7 @@
     </row>
     <row r="215">
       <c r="A215" t="s" s="2">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" t="s" s="2">
@@ -26815,17 +26801,19 @@
         <v>44</v>
       </c>
       <c r="J215" t="s" s="2">
-        <v>192</v>
+        <v>430</v>
       </c>
       <c r="K215" t="s" s="2">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="L215" t="s" s="2">
-        <v>551</v>
-      </c>
-      <c r="M215" s="2"/>
+        <v>562</v>
+      </c>
+      <c r="M215" t="s" s="2">
+        <v>563</v>
+      </c>
       <c r="N215" t="s" s="2">
-        <v>552</v>
+        <v>434</v>
       </c>
       <c r="O215" t="s" s="2">
         <v>44</v>
@@ -26850,11 +26838,13 @@
         <v>44</v>
       </c>
       <c r="W215" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X215" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="X215" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="Y215" t="s" s="2">
-        <v>553</v>
+        <v>44</v>
       </c>
       <c r="Z215" t="s" s="2">
         <v>44</v>
@@ -26872,7 +26862,7 @@
         <v>44</v>
       </c>
       <c r="AE215" t="s" s="2">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="AF215" t="s" s="2">
         <v>42</v>
@@ -26887,7 +26877,7 @@
         <v>44</v>
       </c>
       <c r="AJ215" t="s" s="2">
-        <v>554</v>
+        <v>435</v>
       </c>
       <c r="AK215" t="s" s="2">
         <v>147</v>
@@ -26896,7 +26886,7 @@
         <v>44</v>
       </c>
       <c r="AM215" t="s" s="2">
-        <v>555</v>
+        <v>564</v>
       </c>
       <c r="AN215" t="s" s="2">
         <v>44</v>
@@ -26904,7 +26894,7 @@
     </row>
     <row r="216">
       <c r="A216" t="s" s="2">
-        <v>556</v>
+        <v>565</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" t="s" s="2">
@@ -26927,17 +26917,17 @@
         <v>44</v>
       </c>
       <c r="J216" t="s" s="2">
-        <v>421</v>
+        <v>502</v>
       </c>
       <c r="K216" t="s" s="2">
-        <v>557</v>
+        <v>566</v>
       </c>
       <c r="L216" t="s" s="2">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="M216" s="2"/>
       <c r="N216" t="s" s="2">
-        <v>559</v>
+        <v>568</v>
       </c>
       <c r="O216" t="s" s="2">
         <v>44</v>
@@ -26986,7 +26976,7 @@
         <v>44</v>
       </c>
       <c r="AE216" t="s" s="2">
-        <v>556</v>
+        <v>565</v>
       </c>
       <c r="AF216" t="s" s="2">
         <v>42</v>
@@ -27001,7 +26991,7 @@
         <v>44</v>
       </c>
       <c r="AJ216" t="s" s="2">
-        <v>426</v>
+        <v>507</v>
       </c>
       <c r="AK216" t="s" s="2">
         <v>147</v>
@@ -27010,7 +27000,7 @@
         <v>44</v>
       </c>
       <c r="AM216" t="s" s="2">
-        <v>560</v>
+        <v>569</v>
       </c>
       <c r="AN216" t="s" s="2">
         <v>44</v>
@@ -27018,7 +27008,7 @@
     </row>
     <row r="217">
       <c r="A217" t="s" s="2">
-        <v>561</v>
+        <v>570</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" t="s" s="2">
@@ -27029,7 +27019,7 @@
         <v>42</v>
       </c>
       <c r="F217" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G217" t="s" s="2">
         <v>53</v>
@@ -27041,19 +27031,17 @@
         <v>44</v>
       </c>
       <c r="J217" t="s" s="2">
-        <v>430</v>
+        <v>71</v>
       </c>
       <c r="K217" t="s" s="2">
-        <v>562</v>
+        <v>439</v>
       </c>
       <c r="L217" t="s" s="2">
-        <v>563</v>
-      </c>
-      <c r="M217" t="s" s="2">
-        <v>564</v>
-      </c>
+        <v>571</v>
+      </c>
+      <c r="M217" s="2"/>
       <c r="N217" t="s" s="2">
-        <v>434</v>
+        <v>572</v>
       </c>
       <c r="O217" t="s" s="2">
         <v>44</v>
@@ -27078,13 +27066,13 @@
         <v>44</v>
       </c>
       <c r="W217" t="s" s="2">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="X217" t="s" s="2">
-        <v>44</v>
+        <v>443</v>
       </c>
       <c r="Y217" t="s" s="2">
-        <v>44</v>
+        <v>444</v>
       </c>
       <c r="Z217" t="s" s="2">
         <v>44</v>
@@ -27102,13 +27090,13 @@
         <v>44</v>
       </c>
       <c r="AE217" t="s" s="2">
-        <v>561</v>
+        <v>570</v>
       </c>
       <c r="AF217" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG217" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH217" t="s" s="2">
         <v>44</v>
@@ -27117,7 +27105,7 @@
         <v>44</v>
       </c>
       <c r="AJ217" t="s" s="2">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="AK217" t="s" s="2">
         <v>147</v>
@@ -27126,7 +27114,7 @@
         <v>44</v>
       </c>
       <c r="AM217" t="s" s="2">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="AN217" t="s" s="2">
         <v>44</v>
@@ -27134,7 +27122,7 @@
     </row>
     <row r="218">
       <c r="A218" t="s" s="2">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" t="s" s="2">
@@ -27157,17 +27145,17 @@
         <v>44</v>
       </c>
       <c r="J218" t="s" s="2">
-        <v>503</v>
+        <v>575</v>
       </c>
       <c r="K218" t="s" s="2">
-        <v>567</v>
+        <v>576</v>
       </c>
       <c r="L218" t="s" s="2">
-        <v>568</v>
+        <v>577</v>
       </c>
       <c r="M218" s="2"/>
       <c r="N218" t="s" s="2">
-        <v>569</v>
+        <v>578</v>
       </c>
       <c r="O218" t="s" s="2">
         <v>44</v>
@@ -27216,7 +27204,7 @@
         <v>44</v>
       </c>
       <c r="AE218" t="s" s="2">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="AF218" t="s" s="2">
         <v>42</v>
@@ -27225,13 +27213,13 @@
         <v>52</v>
       </c>
       <c r="AH218" t="s" s="2">
-        <v>44</v>
+        <v>579</v>
       </c>
       <c r="AI218" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AJ218" t="s" s="2">
-        <v>508</v>
+        <v>580</v>
       </c>
       <c r="AK218" t="s" s="2">
         <v>147</v>
@@ -27240,7 +27228,7 @@
         <v>44</v>
       </c>
       <c r="AM218" t="s" s="2">
-        <v>570</v>
+        <v>581</v>
       </c>
       <c r="AN218" t="s" s="2">
         <v>44</v>
@@ -27248,7 +27236,7 @@
     </row>
     <row r="219">
       <c r="A219" t="s" s="2">
-        <v>571</v>
+        <v>582</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s" s="2">
@@ -27271,18 +27259,16 @@
         <v>44</v>
       </c>
       <c r="J219" t="s" s="2">
-        <v>71</v>
+        <v>281</v>
       </c>
       <c r="K219" t="s" s="2">
-        <v>439</v>
+        <v>583</v>
       </c>
       <c r="L219" t="s" s="2">
-        <v>572</v>
+        <v>584</v>
       </c>
       <c r="M219" s="2"/>
-      <c r="N219" t="s" s="2">
-        <v>573</v>
-      </c>
+      <c r="N219" s="2"/>
       <c r="O219" t="s" s="2">
         <v>44</v>
       </c>
@@ -27306,13 +27292,13 @@
         <v>44</v>
       </c>
       <c r="W219" t="s" s="2">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="X219" t="s" s="2">
-        <v>443</v>
+        <v>44</v>
       </c>
       <c r="Y219" t="s" s="2">
-        <v>444</v>
+        <v>44</v>
       </c>
       <c r="Z219" t="s" s="2">
         <v>44</v>
@@ -27330,7 +27316,7 @@
         <v>44</v>
       </c>
       <c r="AE219" t="s" s="2">
-        <v>571</v>
+        <v>582</v>
       </c>
       <c r="AF219" t="s" s="2">
         <v>42</v>
@@ -27345,7 +27331,7 @@
         <v>44</v>
       </c>
       <c r="AJ219" t="s" s="2">
-        <v>445</v>
+        <v>585</v>
       </c>
       <c r="AK219" t="s" s="2">
         <v>147</v>
@@ -27354,15 +27340,15 @@
         <v>44</v>
       </c>
       <c r="AM219" t="s" s="2">
-        <v>574</v>
+        <v>44</v>
       </c>
       <c r="AN219" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" t="s" s="2">
@@ -27373,29 +27359,31 @@
         <v>42</v>
       </c>
       <c r="F220" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G220" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H220" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="H220" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="I220" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J220" t="s" s="2">
-        <v>576</v>
+        <v>535</v>
       </c>
       <c r="K220" t="s" s="2">
-        <v>577</v>
+        <v>587</v>
       </c>
       <c r="L220" t="s" s="2">
-        <v>578</v>
-      </c>
-      <c r="M220" s="2"/>
+        <v>588</v>
+      </c>
+      <c r="M220" t="s" s="2">
+        <v>589</v>
+      </c>
       <c r="N220" t="s" s="2">
-        <v>579</v>
+        <v>590</v>
       </c>
       <c r="O220" t="s" s="2">
         <v>44</v>
@@ -27444,7 +27432,7 @@
         <v>44</v>
       </c>
       <c r="AE220" t="s" s="2">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="AF220" t="s" s="2">
         <v>42</v>
@@ -27453,13 +27441,13 @@
         <v>52</v>
       </c>
       <c r="AH220" t="s" s="2">
-        <v>580</v>
+        <v>44</v>
       </c>
       <c r="AI220" t="s" s="2">
-        <v>44</v>
+        <v>591</v>
       </c>
       <c r="AJ220" t="s" s="2">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="AK220" t="s" s="2">
         <v>147</v>
@@ -27468,15 +27456,15 @@
         <v>44</v>
       </c>
       <c r="AM220" t="s" s="2">
-        <v>582</v>
+        <v>44</v>
       </c>
       <c r="AN220" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" t="s" s="2">
@@ -27490,7 +27478,7 @@
         <v>52</v>
       </c>
       <c r="G221" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H221" t="s" s="2">
         <v>44</v>
@@ -27499,13 +27487,13 @@
         <v>44</v>
       </c>
       <c r="J221" t="s" s="2">
-        <v>281</v>
+        <v>143</v>
       </c>
       <c r="K221" t="s" s="2">
-        <v>584</v>
+        <v>144</v>
       </c>
       <c r="L221" t="s" s="2">
-        <v>585</v>
+        <v>145</v>
       </c>
       <c r="M221" s="2"/>
       <c r="N221" s="2"/>
@@ -27556,7 +27544,7 @@
         <v>44</v>
       </c>
       <c r="AE221" t="s" s="2">
-        <v>583</v>
+        <v>146</v>
       </c>
       <c r="AF221" t="s" s="2">
         <v>42</v>
@@ -27571,10 +27559,10 @@
         <v>44</v>
       </c>
       <c r="AJ221" t="s" s="2">
-        <v>586</v>
+        <v>147</v>
       </c>
       <c r="AK221" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL221" t="s" s="2">
         <v>44</v>
@@ -27588,43 +27576,41 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>587</v>
+        <v>594</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" t="s" s="2">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="D222" s="2"/>
       <c r="E222" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F222" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G222" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H222" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I222" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J222" t="s" s="2">
-        <v>536</v>
+        <v>97</v>
       </c>
       <c r="K222" t="s" s="2">
-        <v>588</v>
+        <v>157</v>
       </c>
       <c r="L222" t="s" s="2">
-        <v>589</v>
+        <v>158</v>
       </c>
       <c r="M222" t="s" s="2">
-        <v>590</v>
-      </c>
-      <c r="N222" t="s" s="2">
-        <v>591</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="N222" s="2"/>
       <c r="O222" t="s" s="2">
         <v>44</v>
       </c>
@@ -27672,25 +27658,25 @@
         <v>44</v>
       </c>
       <c r="AE222" t="s" s="2">
-        <v>587</v>
+        <v>150</v>
       </c>
       <c r="AF222" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG222" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH222" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI222" t="s" s="2">
-        <v>592</v>
+        <v>44</v>
       </c>
       <c r="AJ222" t="s" s="2">
-        <v>593</v>
+        <v>147</v>
       </c>
       <c r="AK222" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL222" t="s" s="2">
         <v>44</v>
@@ -27704,38 +27690,40 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" t="s" s="2">
-        <v>44</v>
+        <v>545</v>
       </c>
       <c r="D223" s="2"/>
       <c r="E223" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F223" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G223" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H223" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I223" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J223" t="s" s="2">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="K223" t="s" s="2">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="L223" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M223" s="2"/>
+        <v>546</v>
+      </c>
+      <c r="M223" t="s" s="2">
+        <v>127</v>
+      </c>
       <c r="N223" s="2"/>
       <c r="O223" t="s" s="2">
         <v>44</v>
@@ -27784,13 +27772,13 @@
         <v>44</v>
       </c>
       <c r="AE223" t="s" s="2">
-        <v>146</v>
+        <v>547</v>
       </c>
       <c r="AF223" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG223" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH223" t="s" s="2">
         <v>44</v>
@@ -27799,7 +27787,7 @@
         <v>44</v>
       </c>
       <c r="AJ223" t="s" s="2">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="AK223" t="s" s="2">
         <v>44</v>
@@ -27816,18 +27804,18 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" t="s" s="2">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="D224" s="2"/>
       <c r="E224" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F224" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G224" t="s" s="2">
         <v>44</v>
@@ -27836,21 +27824,23 @@
         <v>44</v>
       </c>
       <c r="I224" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J224" t="s" s="2">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="K224" t="s" s="2">
-        <v>157</v>
+        <v>597</v>
       </c>
       <c r="L224" t="s" s="2">
-        <v>158</v>
+        <v>598</v>
       </c>
       <c r="M224" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="N224" s="2"/>
+        <v>599</v>
+      </c>
+      <c r="N224" t="s" s="2">
+        <v>600</v>
+      </c>
       <c r="O224" t="s" s="2">
         <v>44</v>
       </c>
@@ -27874,13 +27864,13 @@
         <v>44</v>
       </c>
       <c r="W224" t="s" s="2">
-        <v>44</v>
+        <v>601</v>
       </c>
       <c r="X224" t="s" s="2">
-        <v>44</v>
+        <v>602</v>
       </c>
       <c r="Y224" t="s" s="2">
-        <v>44</v>
+        <v>603</v>
       </c>
       <c r="Z224" t="s" s="2">
         <v>44</v>
@@ -27898,13 +27888,13 @@
         <v>44</v>
       </c>
       <c r="AE224" t="s" s="2">
-        <v>150</v>
+        <v>596</v>
       </c>
       <c r="AF224" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AG224" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH224" t="s" s="2">
         <v>44</v>
@@ -27913,16 +27903,16 @@
         <v>44</v>
       </c>
       <c r="AJ224" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="AK224" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="AK224" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="AL224" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM224" t="s" s="2">
-        <v>44</v>
+        <v>604</v>
       </c>
       <c r="AN224" t="s" s="2">
         <v>44</v>
@@ -27930,41 +27920,43 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="B225" s="2"/>
       <c r="C225" t="s" s="2">
-        <v>546</v>
+        <v>44</v>
       </c>
       <c r="D225" s="2"/>
       <c r="E225" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F225" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G225" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H225" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I225" t="s" s="2">
         <v>53</v>
       </c>
       <c r="J225" t="s" s="2">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="K225" t="s" s="2">
-        <v>125</v>
+        <v>606</v>
       </c>
       <c r="L225" t="s" s="2">
-        <v>547</v>
+        <v>607</v>
       </c>
       <c r="M225" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="N225" s="2"/>
+        <v>608</v>
+      </c>
+      <c r="N225" t="s" s="2">
+        <v>609</v>
+      </c>
       <c r="O225" t="s" s="2">
         <v>44</v>
       </c>
@@ -27988,13 +27980,13 @@
         <v>44</v>
       </c>
       <c r="W225" t="s" s="2">
-        <v>44</v>
+        <v>601</v>
       </c>
       <c r="X225" t="s" s="2">
-        <v>44</v>
+        <v>610</v>
       </c>
       <c r="Y225" t="s" s="2">
-        <v>44</v>
+        <v>611</v>
       </c>
       <c r="Z225" t="s" s="2">
         <v>44</v>
@@ -28012,13 +28004,13 @@
         <v>44</v>
       </c>
       <c r="AE225" t="s" s="2">
-        <v>548</v>
+        <v>605</v>
       </c>
       <c r="AF225" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG225" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH225" t="s" s="2">
         <v>44</v>
@@ -28027,16 +28019,16 @@
         <v>44</v>
       </c>
       <c r="AJ225" t="s" s="2">
-        <v>95</v>
+        <v>612</v>
       </c>
       <c r="AK225" t="s" s="2">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="AL225" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM225" t="s" s="2">
-        <v>44</v>
+        <v>613</v>
       </c>
       <c r="AN225" t="s" s="2">
         <v>44</v>
@@ -28044,7 +28036,7 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>597</v>
+        <v>614</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" t="s" s="2">
@@ -28052,7 +28044,7 @@
       </c>
       <c r="D226" s="2"/>
       <c r="E226" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F226" t="s" s="2">
         <v>52</v>
@@ -28070,16 +28062,14 @@
         <v>192</v>
       </c>
       <c r="K226" t="s" s="2">
-        <v>598</v>
+        <v>615</v>
       </c>
       <c r="L226" t="s" s="2">
-        <v>599</v>
-      </c>
-      <c r="M226" t="s" s="2">
-        <v>600</v>
-      </c>
+        <v>616</v>
+      </c>
+      <c r="M226" s="2"/>
       <c r="N226" t="s" s="2">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="O226" t="s" s="2">
         <v>44</v>
@@ -28104,13 +28094,13 @@
         <v>44</v>
       </c>
       <c r="W226" t="s" s="2">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="X226" t="s" s="2">
-        <v>603</v>
+        <v>618</v>
       </c>
       <c r="Y226" t="s" s="2">
-        <v>604</v>
+        <v>619</v>
       </c>
       <c r="Z226" t="s" s="2">
         <v>44</v>
@@ -28128,10 +28118,10 @@
         <v>44</v>
       </c>
       <c r="AE226" t="s" s="2">
-        <v>597</v>
+        <v>614</v>
       </c>
       <c r="AF226" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AG226" t="s" s="2">
         <v>52</v>
@@ -28143,7 +28133,7 @@
         <v>44</v>
       </c>
       <c r="AJ226" t="s" s="2">
-        <v>554</v>
+        <v>620</v>
       </c>
       <c r="AK226" t="s" s="2">
         <v>147</v>
@@ -28152,15 +28142,15 @@
         <v>44</v>
       </c>
       <c r="AM226" t="s" s="2">
-        <v>605</v>
+        <v>95</v>
       </c>
       <c r="AN226" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="227" hidden="true">
+    <row r="227">
       <c r="A227" t="s" s="2">
-        <v>606</v>
+        <v>621</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" t="s" s="2">
@@ -28171,31 +28161,31 @@
         <v>42</v>
       </c>
       <c r="F227" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G227" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H227" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I227" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J227" t="s" s="2">
-        <v>192</v>
+        <v>535</v>
       </c>
       <c r="K227" t="s" s="2">
-        <v>607</v>
+        <v>622</v>
       </c>
       <c r="L227" t="s" s="2">
-        <v>608</v>
+        <v>623</v>
       </c>
       <c r="M227" t="s" s="2">
-        <v>609</v>
+        <v>624</v>
       </c>
       <c r="N227" t="s" s="2">
-        <v>610</v>
+        <v>625</v>
       </c>
       <c r="O227" t="s" s="2">
         <v>44</v>
@@ -28220,13 +28210,13 @@
         <v>44</v>
       </c>
       <c r="W227" t="s" s="2">
-        <v>602</v>
+        <v>44</v>
       </c>
       <c r="X227" t="s" s="2">
-        <v>611</v>
+        <v>44</v>
       </c>
       <c r="Y227" t="s" s="2">
-        <v>612</v>
+        <v>44</v>
       </c>
       <c r="Z227" t="s" s="2">
         <v>44</v>
@@ -28244,31 +28234,31 @@
         <v>44</v>
       </c>
       <c r="AE227" t="s" s="2">
-        <v>606</v>
+        <v>621</v>
       </c>
       <c r="AF227" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG227" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH227" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI227" t="s" s="2">
-        <v>44</v>
+        <v>591</v>
       </c>
       <c r="AJ227" t="s" s="2">
-        <v>613</v>
+        <v>626</v>
       </c>
       <c r="AK227" t="s" s="2">
-        <v>147</v>
+        <v>627</v>
       </c>
       <c r="AL227" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM227" t="s" s="2">
-        <v>614</v>
+        <v>44</v>
       </c>
       <c r="AN227" t="s" s="2">
         <v>44</v>
@@ -28276,7 +28266,7 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>615</v>
+        <v>628</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" t="s" s="2">
@@ -28296,21 +28286,19 @@
         <v>44</v>
       </c>
       <c r="I228" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J228" t="s" s="2">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="K228" t="s" s="2">
-        <v>616</v>
+        <v>144</v>
       </c>
       <c r="L228" t="s" s="2">
-        <v>617</v>
+        <v>145</v>
       </c>
       <c r="M228" s="2"/>
-      <c r="N228" t="s" s="2">
-        <v>618</v>
-      </c>
+      <c r="N228" s="2"/>
       <c r="O228" t="s" s="2">
         <v>44</v>
       </c>
@@ -28334,13 +28322,13 @@
         <v>44</v>
       </c>
       <c r="W228" t="s" s="2">
-        <v>602</v>
+        <v>44</v>
       </c>
       <c r="X228" t="s" s="2">
-        <v>619</v>
+        <v>44</v>
       </c>
       <c r="Y228" t="s" s="2">
-        <v>620</v>
+        <v>44</v>
       </c>
       <c r="Z228" t="s" s="2">
         <v>44</v>
@@ -28358,7 +28346,7 @@
         <v>44</v>
       </c>
       <c r="AE228" t="s" s="2">
-        <v>615</v>
+        <v>146</v>
       </c>
       <c r="AF228" t="s" s="2">
         <v>42</v>
@@ -28373,28 +28361,28 @@
         <v>44</v>
       </c>
       <c r="AJ228" t="s" s="2">
-        <v>621</v>
+        <v>147</v>
       </c>
       <c r="AK228" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL228" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM228" t="s" s="2">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="AN228" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="B229" s="2"/>
       <c r="C229" t="s" s="2">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="D229" s="2"/>
       <c r="E229" t="s" s="2">
@@ -28404,7 +28392,7 @@
         <v>43</v>
       </c>
       <c r="G229" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H229" t="s" s="2">
         <v>44</v>
@@ -28413,20 +28401,18 @@
         <v>44</v>
       </c>
       <c r="J229" t="s" s="2">
-        <v>536</v>
+        <v>97</v>
       </c>
       <c r="K229" t="s" s="2">
-        <v>623</v>
+        <v>157</v>
       </c>
       <c r="L229" t="s" s="2">
-        <v>624</v>
+        <v>158</v>
       </c>
       <c r="M229" t="s" s="2">
-        <v>625</v>
-      </c>
-      <c r="N229" t="s" s="2">
-        <v>626</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="N229" s="2"/>
       <c r="O229" t="s" s="2">
         <v>44</v>
       </c>
@@ -28474,7 +28460,7 @@
         <v>44</v>
       </c>
       <c r="AE229" t="s" s="2">
-        <v>622</v>
+        <v>150</v>
       </c>
       <c r="AF229" t="s" s="2">
         <v>42</v>
@@ -28486,13 +28472,13 @@
         <v>44</v>
       </c>
       <c r="AI229" t="s" s="2">
-        <v>592</v>
+        <v>44</v>
       </c>
       <c r="AJ229" t="s" s="2">
-        <v>627</v>
+        <v>147</v>
       </c>
       <c r="AK229" t="s" s="2">
-        <v>628</v>
+        <v>44</v>
       </c>
       <c r="AL229" t="s" s="2">
         <v>44</v>
@@ -28506,38 +28492,40 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B230" s="2"/>
       <c r="C230" t="s" s="2">
-        <v>44</v>
+        <v>545</v>
       </c>
       <c r="D230" s="2"/>
       <c r="E230" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F230" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G230" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H230" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I230" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J230" t="s" s="2">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="K230" t="s" s="2">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="L230" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M230" s="2"/>
+        <v>546</v>
+      </c>
+      <c r="M230" t="s" s="2">
+        <v>127</v>
+      </c>
       <c r="N230" s="2"/>
       <c r="O230" t="s" s="2">
         <v>44</v>
@@ -28586,13 +28574,13 @@
         <v>44</v>
       </c>
       <c r="AE230" t="s" s="2">
-        <v>146</v>
+        <v>547</v>
       </c>
       <c r="AF230" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG230" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH230" t="s" s="2">
         <v>44</v>
@@ -28601,7 +28589,7 @@
         <v>44</v>
       </c>
       <c r="AJ230" t="s" s="2">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="AK230" t="s" s="2">
         <v>44</v>
@@ -28616,23 +28604,23 @@
         <v>44</v>
       </c>
     </row>
-    <row r="231" hidden="true">
+    <row r="231">
       <c r="A231" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B231" s="2"/>
       <c r="C231" t="s" s="2">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="D231" s="2"/>
       <c r="E231" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F231" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G231" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H231" t="s" s="2">
         <v>44</v>
@@ -28641,18 +28629,20 @@
         <v>44</v>
       </c>
       <c r="J231" t="s" s="2">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="K231" t="s" s="2">
-        <v>157</v>
+        <v>632</v>
       </c>
       <c r="L231" t="s" s="2">
-        <v>158</v>
+        <v>633</v>
       </c>
       <c r="M231" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="N231" s="2"/>
+        <v>634</v>
+      </c>
+      <c r="N231" t="s" s="2">
+        <v>635</v>
+      </c>
       <c r="O231" t="s" s="2">
         <v>44</v>
       </c>
@@ -28676,13 +28666,11 @@
         <v>44</v>
       </c>
       <c r="W231" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X231" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="X231" s="2"/>
       <c r="Y231" t="s" s="2">
-        <v>44</v>
+        <v>636</v>
       </c>
       <c r="Z231" t="s" s="2">
         <v>44</v>
@@ -28700,13 +28688,13 @@
         <v>44</v>
       </c>
       <c r="AE231" t="s" s="2">
-        <v>150</v>
+        <v>631</v>
       </c>
       <c r="AF231" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AG231" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH231" t="s" s="2">
         <v>44</v>
@@ -28715,58 +28703,60 @@
         <v>44</v>
       </c>
       <c r="AJ231" t="s" s="2">
-        <v>147</v>
+        <v>637</v>
       </c>
       <c r="AK231" t="s" s="2">
-        <v>44</v>
+        <v>638</v>
       </c>
       <c r="AL231" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM231" t="s" s="2">
-        <v>44</v>
+        <v>639</v>
       </c>
       <c r="AN231" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="232" hidden="true">
+    <row r="232">
       <c r="A232" t="s" s="2">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="B232" s="2"/>
       <c r="C232" t="s" s="2">
-        <v>546</v>
+        <v>44</v>
       </c>
       <c r="D232" s="2"/>
       <c r="E232" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F232" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G232" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H232" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I232" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J232" t="s" s="2">
-        <v>97</v>
+        <v>245</v>
       </c>
       <c r="K232" t="s" s="2">
-        <v>125</v>
+        <v>641</v>
       </c>
       <c r="L232" t="s" s="2">
-        <v>547</v>
+        <v>642</v>
       </c>
       <c r="M232" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="N232" s="2"/>
+        <v>643</v>
+      </c>
+      <c r="N232" t="s" s="2">
+        <v>644</v>
+      </c>
       <c r="O232" t="s" s="2">
         <v>44</v>
       </c>
@@ -28814,13 +28804,13 @@
         <v>44</v>
       </c>
       <c r="AE232" t="s" s="2">
-        <v>548</v>
+        <v>640</v>
       </c>
       <c r="AF232" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG232" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH232" t="s" s="2">
         <v>44</v>
@@ -28829,16 +28819,16 @@
         <v>44</v>
       </c>
       <c r="AJ232" t="s" s="2">
-        <v>95</v>
+        <v>645</v>
       </c>
       <c r="AK232" t="s" s="2">
-        <v>44</v>
+        <v>646</v>
       </c>
       <c r="AL232" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM232" t="s" s="2">
-        <v>44</v>
+        <v>647</v>
       </c>
       <c r="AN232" t="s" s="2">
         <v>44</v>
@@ -28846,18 +28836,20 @@
     </row>
     <row r="233">
       <c r="A233" t="s" s="2">
-        <v>632</v>
+        <v>648</v>
       </c>
       <c r="B233" s="2"/>
       <c r="C233" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D233" s="2"/>
+        <v>649</v>
+      </c>
+      <c r="D233" t="s" s="2">
+        <v>650</v>
+      </c>
       <c r="E233" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F233" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G233" t="s" s="2">
         <v>53</v>
@@ -28869,20 +28861,18 @@
         <v>44</v>
       </c>
       <c r="J233" t="s" s="2">
-        <v>192</v>
+        <v>651</v>
       </c>
       <c r="K233" t="s" s="2">
-        <v>633</v>
+        <v>652</v>
       </c>
       <c r="L233" t="s" s="2">
-        <v>634</v>
+        <v>653</v>
       </c>
       <c r="M233" t="s" s="2">
-        <v>635</v>
-      </c>
-      <c r="N233" t="s" s="2">
-        <v>636</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="N233" s="2"/>
       <c r="O233" t="s" s="2">
         <v>44</v>
       </c>
@@ -28906,11 +28896,13 @@
         <v>44</v>
       </c>
       <c r="W233" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X233" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="X233" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="Y233" t="s" s="2">
-        <v>637</v>
+        <v>44</v>
       </c>
       <c r="Z233" t="s" s="2">
         <v>44</v>
@@ -28928,13 +28920,13 @@
         <v>44</v>
       </c>
       <c r="AE233" t="s" s="2">
-        <v>632</v>
+        <v>648</v>
       </c>
       <c r="AF233" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AG233" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH233" t="s" s="2">
         <v>44</v>
@@ -28943,16 +28935,16 @@
         <v>44</v>
       </c>
       <c r="AJ233" t="s" s="2">
-        <v>638</v>
+        <v>655</v>
       </c>
       <c r="AK233" t="s" s="2">
-        <v>639</v>
+        <v>147</v>
       </c>
       <c r="AL233" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM233" t="s" s="2">
-        <v>640</v>
+        <v>656</v>
       </c>
       <c r="AN233" t="s" s="2">
         <v>44</v>
@@ -28960,13 +28952,15 @@
     </row>
     <row r="234">
       <c r="A234" t="s" s="2">
-        <v>641</v>
+        <v>657</v>
       </c>
       <c r="B234" s="2"/>
       <c r="C234" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D234" s="2"/>
+      <c r="D234" t="s" s="2">
+        <v>658</v>
+      </c>
       <c r="E234" t="s" s="2">
         <v>42</v>
       </c>
@@ -28980,22 +28974,22 @@
         <v>44</v>
       </c>
       <c r="I234" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J234" t="s" s="2">
-        <v>245</v>
+        <v>575</v>
       </c>
       <c r="K234" t="s" s="2">
-        <v>642</v>
+        <v>659</v>
       </c>
       <c r="L234" t="s" s="2">
-        <v>643</v>
+        <v>660</v>
       </c>
       <c r="M234" t="s" s="2">
-        <v>644</v>
+        <v>661</v>
       </c>
       <c r="N234" t="s" s="2">
-        <v>645</v>
+        <v>662</v>
       </c>
       <c r="O234" t="s" s="2">
         <v>44</v>
@@ -29044,7 +29038,7 @@
         <v>44</v>
       </c>
       <c r="AE234" t="s" s="2">
-        <v>641</v>
+        <v>657</v>
       </c>
       <c r="AF234" t="s" s="2">
         <v>42</v>
@@ -29059,32 +29053,30 @@
         <v>44</v>
       </c>
       <c r="AJ234" t="s" s="2">
-        <v>646</v>
+        <v>580</v>
       </c>
       <c r="AK234" t="s" s="2">
-        <v>647</v>
+        <v>663</v>
       </c>
       <c r="AL234" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM234" t="s" s="2">
-        <v>648</v>
+        <v>44</v>
       </c>
       <c r="AN234" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>649</v>
+        <v>664</v>
       </c>
       <c r="B235" s="2"/>
       <c r="C235" t="s" s="2">
-        <v>650</v>
-      </c>
-      <c r="D235" t="s" s="2">
-        <v>651</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D235" s="2"/>
       <c r="E235" t="s" s="2">
         <v>42</v>
       </c>
@@ -29092,27 +29084,29 @@
         <v>43</v>
       </c>
       <c r="G235" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H235" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="H235" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="I235" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J235" t="s" s="2">
-        <v>652</v>
+        <v>535</v>
       </c>
       <c r="K235" t="s" s="2">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="L235" t="s" s="2">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="M235" t="s" s="2">
-        <v>655</v>
-      </c>
-      <c r="N235" s="2"/>
+        <v>667</v>
+      </c>
+      <c r="N235" t="s" s="2">
+        <v>668</v>
+      </c>
       <c r="O235" t="s" s="2">
         <v>44</v>
       </c>
@@ -29160,7 +29154,7 @@
         <v>44</v>
       </c>
       <c r="AE235" t="s" s="2">
-        <v>649</v>
+        <v>664</v>
       </c>
       <c r="AF235" t="s" s="2">
         <v>42</v>
@@ -29172,10 +29166,10 @@
         <v>44</v>
       </c>
       <c r="AI235" t="s" s="2">
-        <v>44</v>
+        <v>591</v>
       </c>
       <c r="AJ235" t="s" s="2">
-        <v>656</v>
+        <v>669</v>
       </c>
       <c r="AK235" t="s" s="2">
         <v>147</v>
@@ -29184,23 +29178,21 @@
         <v>44</v>
       </c>
       <c r="AM235" t="s" s="2">
-        <v>657</v>
+        <v>44</v>
       </c>
       <c r="AN235" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
-        <v>658</v>
+        <v>670</v>
       </c>
       <c r="B236" s="2"/>
       <c r="C236" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D236" t="s" s="2">
-        <v>659</v>
-      </c>
+      <c r="D236" s="2"/>
       <c r="E236" t="s" s="2">
         <v>42</v>
       </c>
@@ -29208,29 +29200,25 @@
         <v>52</v>
       </c>
       <c r="G236" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H236" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I236" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J236" t="s" s="2">
-        <v>576</v>
+        <v>143</v>
       </c>
       <c r="K236" t="s" s="2">
-        <v>660</v>
+        <v>144</v>
       </c>
       <c r="L236" t="s" s="2">
-        <v>661</v>
-      </c>
-      <c r="M236" t="s" s="2">
-        <v>662</v>
-      </c>
-      <c r="N236" t="s" s="2">
-        <v>663</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="M236" s="2"/>
+      <c r="N236" s="2"/>
       <c r="O236" t="s" s="2">
         <v>44</v>
       </c>
@@ -29278,7 +29266,7 @@
         <v>44</v>
       </c>
       <c r="AE236" t="s" s="2">
-        <v>658</v>
+        <v>146</v>
       </c>
       <c r="AF236" t="s" s="2">
         <v>42</v>
@@ -29293,10 +29281,10 @@
         <v>44</v>
       </c>
       <c r="AJ236" t="s" s="2">
-        <v>581</v>
+        <v>147</v>
       </c>
       <c r="AK236" t="s" s="2">
-        <v>664</v>
+        <v>44</v>
       </c>
       <c r="AL236" t="s" s="2">
         <v>44</v>
@@ -29310,11 +29298,11 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="B237" s="2"/>
       <c r="C237" t="s" s="2">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="D237" s="2"/>
       <c r="E237" t="s" s="2">
@@ -29327,26 +29315,24 @@
         <v>44</v>
       </c>
       <c r="H237" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I237" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J237" t="s" s="2">
-        <v>536</v>
+        <v>97</v>
       </c>
       <c r="K237" t="s" s="2">
-        <v>666</v>
+        <v>157</v>
       </c>
       <c r="L237" t="s" s="2">
-        <v>667</v>
+        <v>158</v>
       </c>
       <c r="M237" t="s" s="2">
-        <v>668</v>
-      </c>
-      <c r="N237" t="s" s="2">
-        <v>669</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="N237" s="2"/>
       <c r="O237" t="s" s="2">
         <v>44</v>
       </c>
@@ -29394,7 +29380,7 @@
         <v>44</v>
       </c>
       <c r="AE237" t="s" s="2">
-        <v>665</v>
+        <v>150</v>
       </c>
       <c r="AF237" t="s" s="2">
         <v>42</v>
@@ -29406,13 +29392,13 @@
         <v>44</v>
       </c>
       <c r="AI237" t="s" s="2">
-        <v>592</v>
+        <v>44</v>
       </c>
       <c r="AJ237" t="s" s="2">
-        <v>670</v>
+        <v>147</v>
       </c>
       <c r="AK237" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="AL237" t="s" s="2">
         <v>44</v>
@@ -29426,38 +29412,40 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B238" s="2"/>
       <c r="C238" t="s" s="2">
-        <v>44</v>
+        <v>545</v>
       </c>
       <c r="D238" s="2"/>
       <c r="E238" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F238" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G238" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H238" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I238" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J238" t="s" s="2">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="K238" t="s" s="2">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="L238" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M238" s="2"/>
+        <v>546</v>
+      </c>
+      <c r="M238" t="s" s="2">
+        <v>127</v>
+      </c>
       <c r="N238" s="2"/>
       <c r="O238" t="s" s="2">
         <v>44</v>
@@ -29506,13 +29494,13 @@
         <v>44</v>
       </c>
       <c r="AE238" t="s" s="2">
-        <v>146</v>
+        <v>547</v>
       </c>
       <c r="AF238" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG238" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH238" t="s" s="2">
         <v>44</v>
@@ -29521,7 +29509,7 @@
         <v>44</v>
       </c>
       <c r="AJ238" t="s" s="2">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="AK238" t="s" s="2">
         <v>44</v>
@@ -29538,18 +29526,18 @@
     </row>
     <row r="239" hidden="true">
       <c r="A239" t="s" s="2">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B239" s="2"/>
       <c r="C239" t="s" s="2">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="D239" s="2"/>
       <c r="E239" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F239" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G239" t="s" s="2">
         <v>44</v>
@@ -29558,19 +29546,19 @@
         <v>44</v>
       </c>
       <c r="I239" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J239" t="s" s="2">
-        <v>97</v>
+        <v>674</v>
       </c>
       <c r="K239" t="s" s="2">
-        <v>157</v>
+        <v>675</v>
       </c>
       <c r="L239" t="s" s="2">
-        <v>158</v>
+        <v>676</v>
       </c>
       <c r="M239" t="s" s="2">
-        <v>127</v>
+        <v>677</v>
       </c>
       <c r="N239" s="2"/>
       <c r="O239" t="s" s="2">
@@ -29620,13 +29608,13 @@
         <v>44</v>
       </c>
       <c r="AE239" t="s" s="2">
-        <v>150</v>
+        <v>673</v>
       </c>
       <c r="AF239" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AG239" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH239" t="s" s="2">
         <v>44</v>
@@ -29635,16 +29623,16 @@
         <v>44</v>
       </c>
       <c r="AJ239" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AK239" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="AK239" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="AL239" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM239" t="s" s="2">
-        <v>44</v>
+        <v>678</v>
       </c>
       <c r="AN239" t="s" s="2">
         <v>44</v>
@@ -29652,40 +29640,38 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="B240" s="2"/>
       <c r="C240" t="s" s="2">
-        <v>546</v>
+        <v>44</v>
       </c>
       <c r="D240" s="2"/>
       <c r="E240" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F240" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G240" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H240" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I240" t="s" s="2">
         <v>53</v>
       </c>
       <c r="J240" t="s" s="2">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="K240" t="s" s="2">
-        <v>125</v>
+        <v>680</v>
       </c>
       <c r="L240" t="s" s="2">
-        <v>547</v>
-      </c>
-      <c r="M240" t="s" s="2">
-        <v>127</v>
-      </c>
+        <v>681</v>
+      </c>
+      <c r="M240" s="2"/>
       <c r="N240" s="2"/>
       <c r="O240" t="s" s="2">
         <v>44</v>
@@ -29710,13 +29696,13 @@
         <v>44</v>
       </c>
       <c r="W240" t="s" s="2">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="X240" t="s" s="2">
-        <v>44</v>
+        <v>681</v>
       </c>
       <c r="Y240" t="s" s="2">
-        <v>44</v>
+        <v>682</v>
       </c>
       <c r="Z240" t="s" s="2">
         <v>44</v>
@@ -29734,13 +29720,13 @@
         <v>44</v>
       </c>
       <c r="AE240" t="s" s="2">
-        <v>548</v>
+        <v>679</v>
       </c>
       <c r="AF240" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AG240" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH240" t="s" s="2">
         <v>44</v>
@@ -29749,10 +29735,10 @@
         <v>44</v>
       </c>
       <c r="AJ240" t="s" s="2">
-        <v>95</v>
+        <v>683</v>
       </c>
       <c r="AK240" t="s" s="2">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="AL240" t="s" s="2">
         <v>44</v>
@@ -29761,237 +29747,11 @@
         <v>44</v>
       </c>
       <c r="AN240" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="241" hidden="true">
-      <c r="A241" t="s" s="2">
-        <v>674</v>
-      </c>
-      <c r="B241" s="2"/>
-      <c r="C241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D241" s="2"/>
-      <c r="E241" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F241" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I241" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J241" t="s" s="2">
-        <v>675</v>
-      </c>
-      <c r="K241" t="s" s="2">
-        <v>676</v>
-      </c>
-      <c r="L241" t="s" s="2">
-        <v>677</v>
-      </c>
-      <c r="M241" t="s" s="2">
-        <v>678</v>
-      </c>
-      <c r="N241" s="2"/>
-      <c r="O241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P241" s="2"/>
-      <c r="Q241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE241" t="s" s="2">
-        <v>674</v>
-      </c>
-      <c r="AF241" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG241" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ241" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="AK241" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="AL241" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM241" t="s" s="2">
-        <v>679</v>
-      </c>
-      <c r="AN241" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="242" hidden="true">
-      <c r="A242" t="s" s="2">
-        <v>680</v>
-      </c>
-      <c r="B242" s="2"/>
-      <c r="C242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D242" s="2"/>
-      <c r="E242" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F242" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I242" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J242" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="K242" t="s" s="2">
-        <v>681</v>
-      </c>
-      <c r="L242" t="s" s="2">
-        <v>682</v>
-      </c>
-      <c r="M242" s="2"/>
-      <c r="N242" s="2"/>
-      <c r="O242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P242" s="2"/>
-      <c r="Q242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W242" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="X242" t="s" s="2">
-        <v>682</v>
-      </c>
-      <c r="Y242" t="s" s="2">
-        <v>683</v>
-      </c>
-      <c r="Z242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE242" t="s" s="2">
-        <v>680</v>
-      </c>
-      <c r="AF242" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG242" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ242" t="s" s="2">
-        <v>684</v>
-      </c>
-      <c r="AK242" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="AL242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM242" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN242" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN242">
+  <autoFilter ref="A1:AN240">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -30001,7 +29761,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI241">
+  <conditionalFormatting sqref="A2:AI239">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>